<commit_message>
train model and select model
</commit_message>
<xml_diff>
--- a/modeling/report/01-eda.xlsx
+++ b/modeling/report/01-eda.xlsx
@@ -515,10 +515,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E2" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F2" t="n">
         <v>2</v>
@@ -559,10 +559,10 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E3" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F3" t="n">
         <v>2</v>
@@ -603,10 +603,10 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E4" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F4" t="n">
         <v>2</v>
@@ -647,10 +647,10 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E5" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F5" t="n">
         <v>2</v>
@@ -691,10 +691,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E6" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F6" t="n">
         <v>73</v>
@@ -712,7 +712,7 @@
         <v>72</v>
       </c>
       <c r="K6" t="n">
-        <v>32.38</v>
+        <v>32.37</v>
       </c>
       <c r="L6" t="n">
         <v>24.56</v>
@@ -743,10 +743,10 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E7" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F7" t="n">
         <v>2</v>
@@ -787,10 +787,10 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E8" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F8" t="n">
         <v>3</v>
@@ -831,10 +831,10 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E9" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F9" t="n">
         <v>3</v>
@@ -875,10 +875,10 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E10" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F10" t="n">
         <v>3</v>
@@ -919,10 +919,10 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E11" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F11" t="n">
         <v>3</v>
@@ -963,10 +963,10 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E12" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F12" t="n">
         <v>3</v>
@@ -1007,10 +1007,10 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E13" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F13" t="n">
         <v>3</v>
@@ -1051,10 +1051,10 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E14" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F14" t="n">
         <v>3</v>
@@ -1095,10 +1095,10 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E15" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F15" t="n">
         <v>3</v>
@@ -1139,10 +1139,10 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E16" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F16" t="n">
         <v>3</v>
@@ -1183,10 +1183,10 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E17" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F17" t="n">
         <v>2</v>
@@ -1227,10 +1227,10 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E18" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F18" t="n">
         <v>4</v>
@@ -1271,10 +1271,10 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E19" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F19" t="n">
         <v>1585</v>
@@ -1292,7 +1292,7 @@
         <v>118.75</v>
       </c>
       <c r="K19" t="n">
-        <v>64.77</v>
+        <v>64.76000000000001</v>
       </c>
       <c r="L19" t="n">
         <v>30.09</v>
@@ -1323,13 +1323,13 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E20" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F20" t="n">
-        <v>6530</v>
+        <v>6531</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
@@ -1344,10 +1344,10 @@
         <v>8684.799999999999</v>
       </c>
       <c r="K20" t="n">
-        <v>2282.64</v>
+        <v>2281.92</v>
       </c>
       <c r="L20" t="n">
-        <v>2265.92</v>
+        <v>2265.27</v>
       </c>
       <c r="M20" t="inlineStr">
         <is>
@@ -1375,10 +1375,10 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="E21" t="n">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F21" t="n">
         <v>2</v>

</xml_diff>